<commit_message>
clefig titles changed letters to capitalized
</commit_message>
<xml_diff>
--- a/data/rot-experiment/algae-rot-summaries-larry-08.06.21.xlsx
+++ b/data/rot-experiment/algae-rot-summaries-larry-08.06.21.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="82">
   <si>
     <t xml:space="preserve">Second Algal Rot Flask Experiment</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t xml:space="preserve">Dissolved Carbon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Megan’s calcs</t>
   </si>
   <si>
     <t xml:space="preserve">(whole cells)</t>
@@ -188,6 +191,15 @@
     <t xml:space="preserve">BAC-PRO/</t>
   </si>
   <si>
+    <t xml:space="preserve">Bac:Algal cell ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C/Bac cell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C/Alg cell</t>
+  </si>
+  <si>
     <t xml:space="preserve">Time (days)</t>
   </si>
   <si>
@@ -245,10 +257,16 @@
     <t xml:space="preserve">µm3</t>
   </si>
   <si>
+    <t xml:space="preserve">mg C/cell</t>
+  </si>
+  <si>
     <t xml:space="preserve">N.D.</t>
   </si>
   <si>
     <t xml:space="preserve">Washed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">average</t>
   </si>
   <si>
     <t xml:space="preserve">Resuspend</t>
@@ -662,12 +680,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:AK238"/>
+  <dimension ref="A1:AN238"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="1768" ySplit="0" topLeftCell="W1" activePane="topRight" state="split"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="AJ75" activeCellId="0" sqref="AJ75"/>
+      <selection pane="topRight" activeCell="AN18" activeCellId="0" sqref="AN18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.16015625" defaultRowHeight="13" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -697,7 +715,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="3" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="3" width="6.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="3" width="7.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="8.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="15.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="5" width="6"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="6" width="9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="9.16"/>
@@ -720,7 +738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
@@ -743,222 +761,240 @@
         <v>8</v>
       </c>
       <c r="U3" s="9"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AL3" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G4" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J4" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N4" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P4" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q4" s="15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R4" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V4" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="W4" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="X4" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Y4" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Z4" s="16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AA4" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AB4" s="18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AC4" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AD4" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AE4" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AF4" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AG4" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AH4" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AI4" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AJ4" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AK4" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>42</v>
+      </c>
+      <c r="AL4" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="AM4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN4" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="19" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F5" s="10"/>
       <c r="G5" s="21" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="K5" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="L5" s="21"/>
       <c r="M5" s="21" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="N5" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="O5" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="P5" s="23" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="Q5" s="24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R5" s="24" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="S5" s="21" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="T5" s="10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="U5" s="10" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="V5" s="23" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="W5" s="25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="X5" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="Y5" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="Z5" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AA5" s="26" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="AB5" s="27" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="AC5" s="24"/>
       <c r="AD5" s="28" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="AE5" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AG5" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AH5" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AI5" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="AJ5" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AK5" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>55</v>
+      </c>
+      <c r="AM5" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="AN5" s="0" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="n">
         <v>0</v>
       </c>
@@ -1070,10 +1106,22 @@
         <v>8.58944324654816E-010</v>
       </c>
       <c r="AI6" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+      <c r="AL6" s="0" t="n">
+        <f aca="false">AA6/AD6</f>
+        <v>0.091644204851752</v>
+      </c>
+      <c r="AM6" s="0" t="n">
+        <f aca="false">AB6/AA6</f>
+        <v>0</v>
+      </c>
+      <c r="AN6" s="0" t="n">
+        <f aca="false">B6/AD6</f>
+        <v>1.34584007187781E-008</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="n">
         <v>0</v>
       </c>
@@ -1187,10 +1235,22 @@
         <v>2.5064303368193E-010</v>
       </c>
       <c r="AI7" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+      <c r="AL7" s="0" t="n">
+        <f aca="false">AA7/AD7</f>
+        <v>0.307511737089202</v>
+      </c>
+      <c r="AM7" s="0" t="n">
+        <f aca="false">AB7/AA7</f>
+        <v>0</v>
+      </c>
+      <c r="AN7" s="0" t="n">
+        <f aca="false">B7/AD7</f>
+        <v>1.1468544600939E-008</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="n">
         <v>0.3</v>
       </c>
@@ -1309,10 +1369,22 @@
         <v>1.46751317355717E-009</v>
       </c>
       <c r="AI8" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>66</v>
+      </c>
+      <c r="AL8" s="0" t="n">
+        <f aca="false">AA8/AD8</f>
+        <v>0.152963671128107</v>
+      </c>
+      <c r="AM8" s="0" t="n">
+        <f aca="false">AB8/AA8</f>
+        <v>0</v>
+      </c>
+      <c r="AN8" s="0" t="n">
+        <f aca="false">B8/AD8</f>
+        <v>9.45213511790949E-009</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="n">
         <v>1</v>
       </c>
@@ -1444,8 +1516,20 @@
         <f aca="false">AJ9/J9</f>
         <v>0.236869572729994</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AL9" s="0" t="n">
+        <f aca="false">AA9/AD9</f>
+        <v>462.5</v>
+      </c>
+      <c r="AM9" s="0" t="n">
+        <f aca="false">AB9/AA9</f>
+        <v>3.28289358831987E-011</v>
+      </c>
+      <c r="AN9" s="0" t="n">
+        <f aca="false">B9/AD9</f>
+        <v>8.34666666666667E-008</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
         <v>2</v>
       </c>
@@ -1577,8 +1661,16 @@
         <f aca="false">AJ10/J10</f>
         <v>0.392861472179189</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AL10" s="0" t="e">
+        <f aca="false">AA10/AD10</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AM10" s="0" t="n">
+        <f aca="false">AB10/AA10</f>
+        <v>2.5844192243093E-011</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="n">
         <v>3</v>
       </c>
@@ -1710,8 +1802,16 @@
         <f aca="false">AJ11/J11</f>
         <v>0.304186949151696</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AL11" s="0" t="e">
+        <f aca="false">AA11/AD11</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AM11" s="0" t="n">
+        <f aca="false">AB11/AA11</f>
+        <v>2.67853321843725E-011</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
         <v>4</v>
       </c>
@@ -1843,8 +1943,16 @@
         <f aca="false">AJ12/J12</f>
         <v>0.264212285956304</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AL12" s="0" t="n">
+        <f aca="false">AA12/AD12</f>
+        <v>1108.71428571429</v>
+      </c>
+      <c r="AM12" s="0" t="n">
+        <f aca="false">AB12/AA12</f>
+        <v>2.86020260392994E-011</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="n">
         <v>6</v>
       </c>
@@ -1976,8 +2084,16 @@
         <f aca="false">AJ13/J13</f>
         <v>0.322420357100658</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AL13" s="0" t="n">
+        <f aca="false">AA13/AD13</f>
+        <v>1260</v>
+      </c>
+      <c r="AM13" s="0" t="n">
+        <f aca="false">AB13/AA13</f>
+        <v>3.03418150683309E-011</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="n">
         <v>9</v>
       </c>
@@ -2109,8 +2225,16 @@
         <f aca="false">AJ14/J14</f>
         <v>0.172493110590027</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AL14" s="0" t="e">
+        <f aca="false">AA14/AD14</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AM14" s="0" t="n">
+        <f aca="false">AB14/AA14</f>
+        <v>2.48786044931374E-011</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="n">
         <v>12</v>
       </c>
@@ -2242,8 +2366,16 @@
         <f aca="false">AJ15/J15</f>
         <v>0.228166052549262</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AL15" s="0" t="e">
+        <f aca="false">AA15/AD15</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AM15" s="0" t="n">
+        <f aca="false">AB15/AA15</f>
+        <v>2.48786044931374E-011</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
         <v>19</v>
       </c>
@@ -2375,8 +2507,16 @@
         <f aca="false">AJ16/J16</f>
         <v>0.172281683535388</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AL16" s="0" t="e">
+        <f aca="false">AA16/AD16</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AM16" s="0" t="n">
+        <f aca="false">AB16/AA16</f>
+        <v>2.3886235740941E-011</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="n">
         <v>28</v>
       </c>
@@ -2508,10 +2648,18 @@
         <f aca="false">AJ17/J17</f>
         <v>0.0697442082593047</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AL17" s="0" t="e">
+        <f aca="false">AA17/AD17</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AM17" s="0" t="n">
+        <f aca="false">AB17/AA17</f>
+        <v>2.1809670699945E-011</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="G18" s="2" t="n">
         <v>34.7148226533525</v>
@@ -2538,10 +2686,21 @@
         <v>1</v>
       </c>
       <c r="AK18" s="29"/>
+      <c r="AL18" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="AM18" s="0" t="n">
+        <f aca="false">AVERAGE(AM9:AM17)</f>
+        <v>2.66506018717173E-011</v>
+      </c>
+      <c r="AN18" s="0" t="n">
+        <f aca="false">AVERAGE(AN6:AN9)</f>
+        <v>2.94614367760733E-008</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G19" s="2" t="n">
         <v>28.2374715127391</v>
@@ -2578,7 +2737,7 @@
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>3</v>
@@ -2607,186 +2766,186 @@
     </row>
     <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G22" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J22" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N22" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P22" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q22" s="15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R22" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="U22" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V22" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="W22" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="X22" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Y22" s="16"/>
       <c r="Z22" s="16"/>
       <c r="AA22" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AB22" s="18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AC22" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AD22" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AE22" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AF22" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AG22" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AH22" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AI22" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AK22" s="29"/>
     </row>
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="19" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G23" s="21" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H23" s="10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="J23" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="K23" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="L23" s="21"/>
       <c r="M23" s="21"/>
       <c r="N23" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="O23" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="P23" s="23" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="Q23" s="24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R23" s="24" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="S23" s="21" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="T23" s="10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="U23" s="10" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="V23" s="23" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="W23" s="25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="X23" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="AA23" s="26" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="AB23" s="27" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="AC23" s="24"/>
       <c r="AD23" s="28" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="AE23" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AG23" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AH23" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AI23" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="AK23" s="29"/>
     </row>
@@ -2851,7 +3010,7 @@
         <v>1.84472796029058E-010</v>
       </c>
       <c r="AI24" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AK24" s="29"/>
     </row>
@@ -2916,7 +3075,7 @@
         <v>1.44464987369706E-010</v>
       </c>
       <c r="AI25" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AK25" s="29"/>
     </row>
@@ -2981,7 +3140,7 @@
         <v>2.98689731208929E-010</v>
       </c>
       <c r="AI26" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AK26" s="29"/>
     </row>
@@ -3046,7 +3205,7 @@
         <v>6.55375259434108E-011</v>
       </c>
       <c r="AI27" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AK27" s="29"/>
     </row>
@@ -3114,7 +3273,7 @@
         <v>9.26475637070977E-012</v>
       </c>
       <c r="AI28" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AK28" s="29"/>
     </row>
@@ -3179,7 +3338,7 @@
         <v>3.01835083425382E-010</v>
       </c>
       <c r="AI29" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AJ29" s="2" t="s">
         <v>1</v>
@@ -3247,7 +3406,7 @@
         <v>4.87962962962963E-010</v>
       </c>
       <c r="AI30" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AK30" s="29"/>
     </row>
@@ -3308,7 +3467,7 @@
         <v>0</v>
       </c>
       <c r="AI31" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AK31" s="29"/>
     </row>
@@ -3369,7 +3528,7 @@
         <v>0</v>
       </c>
       <c r="AI32" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AK32" s="29"/>
     </row>
@@ -3430,7 +3589,7 @@
         <v>0</v>
       </c>
       <c r="AI33" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AK33" s="29"/>
     </row>
@@ -3491,7 +3650,7 @@
         <v>0</v>
       </c>
       <c r="AI34" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AK34" s="29"/>
     </row>
@@ -3552,7 +3711,7 @@
         <v>0</v>
       </c>
       <c r="AI35" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AK35" s="29"/>
     </row>
@@ -3561,7 +3720,7 @@
         <v>28</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G36" s="2" t="n">
         <v>17.6</v>
@@ -3599,7 +3758,7 @@
     </row>
     <row r="37" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B37" s="3"/>
       <c r="G37" s="34" t="n">
@@ -3619,7 +3778,7 @@
     </row>
     <row r="38" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="B38" s="3"/>
       <c r="G38" s="34" t="n">
@@ -3661,7 +3820,7 @@
     </row>
     <row r="40" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="H40" s="2" t="s">
         <v>4</v>
@@ -3687,210 +3846,210 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E41" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J41" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K41" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L41" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N41" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P41" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q41" s="15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R41" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S41" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="T41" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="U41" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V41" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="W41" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="X41" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Y41" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Z41" s="16" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="AA41" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AB41" s="18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AC41" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AD41" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AE41" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AF41" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AG41" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AH41" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AI41" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AJ41" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AK41" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="19" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E42" s="10" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="F42" s="10"/>
       <c r="G42" s="21" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H42" s="10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I42" s="22" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="J42" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="K42" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="L42" s="21"/>
       <c r="M42" s="21" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="N42" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="O42" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="P42" s="23" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="Q42" s="24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R42" s="24" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="S42" s="21" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="T42" s="10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="U42" s="10" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="V42" s="23" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="W42" s="25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="X42" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="Y42" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AA42" s="26" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="AB42" s="27" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="AC42" s="24"/>
       <c r="AD42" s="28" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="AE42" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AG42" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AH42" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AI42" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="AJ42" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AK42" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4005,7 +4164,7 @@
         <v>8.15754723574436E-010</v>
       </c>
       <c r="AI43" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AK43" s="29"/>
     </row>
@@ -4121,7 +4280,7 @@
         <v>3.09428393790146E-010</v>
       </c>
       <c r="AI44" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AK44" s="29"/>
     </row>
@@ -4244,7 +4403,7 @@
         <v>1.23375839026733E-009</v>
       </c>
       <c r="AI45" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AK45" s="29"/>
     </row>
@@ -5447,7 +5606,7 @@
     </row>
     <row r="55" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="G55" s="2" t="n">
         <v>51.7976101732677</v>
@@ -5471,7 +5630,7 @@
     </row>
     <row r="56" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G56" s="2" t="n">
         <v>51.9065000167257</v>
@@ -5505,7 +5664,7 @@
     </row>
     <row r="58" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="8" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="C58" s="2" t="s">
         <v>3</v>
@@ -5534,212 +5693,212 @@
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E59" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F59" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G59" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J59" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K59" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L59" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M59" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N59" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O59" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P59" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q59" s="15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R59" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S59" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="T59" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="U59" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V59" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="W59" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="X59" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Y59" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Z59" s="16" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="AA59" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AB59" s="18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AC59" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AD59" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AE59" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AF59" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AG59" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AH59" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AI59" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AJ59" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AK59" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="19" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B60" s="20" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F60" s="10" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G60" s="21" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I60" s="22" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="J60" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="K60" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="L60" s="21"/>
       <c r="M60" s="21" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="N60" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="O60" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="P60" s="23" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="Q60" s="24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R60" s="24" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="S60" s="21" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="T60" s="10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="U60" s="10" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="V60" s="23" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="W60" s="25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="X60" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="Y60" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AA60" s="26" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="AB60" s="27" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="AC60" s="24"/>
       <c r="AD60" s="28" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="AE60" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AG60" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AH60" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AI60" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="AJ60" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AK60" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5854,7 +6013,7 @@
         <v>1.51302350449238E-009</v>
       </c>
       <c r="AI61" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AK61" s="29"/>
     </row>
@@ -5970,7 +6129,7 @@
         <v>6.71310150287882E-010</v>
       </c>
       <c r="AI62" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AK62" s="29"/>
     </row>
@@ -6093,7 +6252,7 @@
         <v>1.15110851739128E-009</v>
       </c>
       <c r="AI63" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AK63" s="29"/>
     </row>
@@ -7296,7 +7455,7 @@
     </row>
     <row r="73" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="G73" s="2" t="n">
         <v>44.3070878714689</v>
@@ -7320,7 +7479,7 @@
     </row>
     <row r="74" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G74" s="2" t="n">
         <v>73.1203199531443</v>
@@ -7360,7 +7519,7 @@
     </row>
     <row r="76" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="8" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="C76" s="2" t="s">
         <v>3</v>
@@ -7389,212 +7548,212 @@
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="0" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E77" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F77" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G77" s="11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H77" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J77" s="12" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K77" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L77" s="13" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M77" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N77" s="11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="O77" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="P77" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Q77" s="15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="R77" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="S77" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="T77" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="U77" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="V77" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="W77" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="X77" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Y77" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Z77" s="16" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="AA77" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AB77" s="18" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AC77" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AD77" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AE77" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AF77" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AG77" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AH77" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AI77" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AJ77" s="2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AK77" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="19" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B78" s="20" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C78" s="10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="F78" s="10" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G78" s="21" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H78" s="10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I78" s="22" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="J78" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="K78" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="L78" s="21"/>
       <c r="M78" s="21" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="N78" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="O78" s="21" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="P78" s="23" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="Q78" s="24" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="R78" s="24" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="S78" s="21" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="T78" s="10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="U78" s="10" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="V78" s="23" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="W78" s="25" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="X78" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="Y78" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="AA78" s="26" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="AB78" s="27" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="AC78" s="24"/>
       <c r="AD78" s="28" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="AE78" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AG78" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AH78" s="0" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AI78" s="3" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="AJ78" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="AK78" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7709,7 +7868,7 @@
         <v>7.13521947181546E-010</v>
       </c>
       <c r="AI79" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AK79" s="29"/>
     </row>
@@ -7825,7 +7984,7 @@
         <v>1.0515816669189E-009</v>
       </c>
       <c r="AI80" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AK80" s="29"/>
     </row>
@@ -7948,7 +8107,7 @@
         <v>6.55874106923212E-010</v>
       </c>
       <c r="AI81" s="3" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="AK81" s="29"/>
     </row>
@@ -9151,7 +9310,7 @@
     </row>
     <row r="91" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="3" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="G91" s="34" t="n">
         <v>68.2777385850946</v>
@@ -9170,7 +9329,7 @@
     </row>
     <row r="92" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="3" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G92" s="34" t="n">
         <v>76.7145506017083</v>

</xml_diff>